<commit_message>
Update changes in inventory include: inbounds upload
</commit_message>
<xml_diff>
--- a/src/assets/documents/FORMATO_ENTRADA.xlsx
+++ b/src/assets/documents/FORMATO_ENTRADA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aemo/Projects/bellarti-app/src/assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207F1267-B9BA-4241-90B7-1679413A2634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881F3F47-E773-5C40-9732-469FA3261AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{6266A802-928D-A74F-8AB8-7325AD93887E}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,13 +75,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -106,10 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +439,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,10 +457,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">

</xml_diff>